<commit_message>
update experiments results with CICDDoS2019 and Random Forest
</commit_message>
<xml_diff>
--- a/Anying Xiang/SEP-B/Sprint 4/Experiment/CICDDoS2019-cv5/Random Forest/response time.xlsx
+++ b/Anying Xiang/SEP-B/Sprint 4/Experiment/CICDDoS2019-cv5/Random Forest/response time.xlsx
@@ -43,57 +43,60 @@
     <t xml:space="preserve">default value</t>
   </si>
   <si>
+    <t xml:space="preserve">10.33.184.108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all default configurations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.33.184.86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spark.executor.cores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spark.io.compression.codec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lzf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lz4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snappy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spark.rdd.compress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spark.serializer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org.apache.spark.serializer.KryoSerializer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JavaSerializer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.33.184.116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spark.io.compression.lz4.blockSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64k</t>
+  </si>
+  <si>
     <t xml:space="preserve">10.33.184.91</t>
   </si>
   <si>
-    <t xml:space="preserve">all default configurations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.33.184.108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spark.executor.cores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spark.io.compression.codec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lzf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lz4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">snappy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spark.rdd.compress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spark.serializer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org.apache.spark.serializer.KryoSerializer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JavaSerializer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.33.184.116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spark.io.compression.lz4.blockSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64k</t>
-  </si>
-  <si>
     <t xml:space="preserve">spark.shuffle.spill.compress</t>
   </si>
   <si>
@@ -125,9 +128,6 @@
   </si>
   <si>
     <t xml:space="preserve">4m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.33.184.86</t>
   </si>
   <si>
     <t xml:space="preserve">8m</t>
@@ -377,7 +377,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -461,81 +461,81 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>140404</c:v>
+                  <c:v>389170</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>111891</c:v>
+                  <c:v>266003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>131234</c:v>
+                  <c:v>386600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>130188</c:v>
+                  <c:v>393378</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>125486</c:v>
+                  <c:v>388956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>146655</c:v>
+                  <c:v>389166</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69737</c:v>
+                  <c:v>388383</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>130473</c:v>
+                  <c:v>393489</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>144139</c:v>
+                  <c:v>342829</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>136136</c:v>
+                  <c:v>390035</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>137986</c:v>
+                  <c:v>384049</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>135457</c:v>
+                  <c:v>335683</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>133922</c:v>
+                  <c:v>379439</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>139746</c:v>
+                  <c:v>395040</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>130484</c:v>
+                  <c:v>385262</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>134970</c:v>
+                  <c:v>386010</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>89207</c:v>
+                  <c:v>359204</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>150244</c:v>
+                  <c:v>341364</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>68113</c:v>
+                  <c:v>401041</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>139568</c:v>
+                  <c:v>349520</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>133947</c:v>
+                  <c:v>392047</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>142900</c:v>
+                  <c:v>384984</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="17805259"/>
-        <c:axId val="67013956"/>
+        <c:axId val="42961853"/>
+        <c:axId val="47108684"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="17805259"/>
+        <c:axId val="42961853"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -611,12 +611,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67013956"/>
+        <c:crossAx val="47108684"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67013956"/>
+        <c:axId val="47108684"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +658,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17805259"/>
+        <c:crossAx val="42961853"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -697,9 +697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>197280</xdr:colOff>
+      <xdr:colOff>196920</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -708,7 +708,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="12106800" y="548640"/>
-        <a:ext cx="3785760" cy="1865880"/>
+        <a:ext cx="3785400" cy="1865520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -729,7 +729,7 @@
   <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -772,10 +772,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>140404</v>
+        <v>389170</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
@@ -791,10 +791,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>111891</v>
+        <v>266003</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -814,13 +814,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>131234</v>
+        <v>386600</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>11</v>
@@ -837,13 +837,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>130188</v>
+        <v>393378</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4" t="s">
@@ -856,10 +856,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>125486</v>
+        <v>388956</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>7</v>
@@ -881,10 +881,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>146655</v>
+        <v>389166</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
@@ -904,10 +904,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>69737</v>
+        <v>388383</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>19</v>
@@ -927,13 +927,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>130473</v>
+        <v>393489</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
@@ -946,16 +946,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>144139</v>
+        <v>342829</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G11" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -971,22 +971,22 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>136136</v>
+        <v>390035</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,17 +994,17 @@
         <v>10</v>
       </c>
       <c r="C13" s="3" t="n">
-        <v>137986</v>
+        <v>384049</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>160</v>
+        <v>85</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H13" s="5"/>
     </row>
@@ -1013,16 +1013,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>135457</v>
+        <v>335683</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>21</v>
@@ -1036,17 +1036,17 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>133922</v>
+        <v>379439</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H15" s="5"/>
     </row>
@@ -1055,16 +1055,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>139746</v>
+        <v>395040</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G16" s="4" t="n">
         <f aca="false">FALSE()</f>
@@ -1080,22 +1080,22 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>130484</v>
+        <v>385262</v>
       </c>
       <c r="D17" s="3" t="n">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,13 +1103,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>134970</v>
+        <v>386010</v>
       </c>
       <c r="D18" s="3" t="n">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
@@ -1122,10 +1122,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>89207</v>
+        <v>359204</v>
       </c>
       <c r="D19" s="3" t="n">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>7</v>
@@ -1145,13 +1145,13 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>150244</v>
+        <v>341364</v>
       </c>
       <c r="D20" s="3" t="n">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
@@ -1164,10 +1164,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>68113</v>
+        <v>401041</v>
       </c>
       <c r="D21" s="3" t="n">
-        <v>169</v>
+        <v>92</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>19</v>
@@ -1187,13 +1187,13 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>139568</v>
+        <v>349520</v>
       </c>
       <c r="D22" s="3" t="n">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="n">
@@ -1206,10 +1206,10 @@
         <v>20</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>133947</v>
+        <v>392047</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
@@ -1229,10 +1229,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>142900</v>
+        <v>384984</v>
       </c>
       <c r="D24" s="3" t="n">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>9</v>

</xml_diff>